<commit_message>
se creo la se finalizo la parte de dar formato a los datos del tipo de corte 2, se creo el formato para reportes con codcli, se empezaron a pintar los datos en el excel
</commit_message>
<xml_diff>
--- a/coediciones.xlsx
+++ b/coediciones.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">
 CORTES DE VENTAS DE COEDICIONES
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t xml:space="preserve">Periodo: Junio 1 de 2023 a Junio 30 de 2023 - VENTAS NACIONALES    </t>
-  </si>
-  <si>
-    <t xml:space="preserve">N.º Corte</t>
   </si>
   <si>
     <t xml:space="preserve">Codigo</t>
@@ -361,9 +358,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1402920</xdr:colOff>
+      <xdr:colOff>1402560</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>111600</xdr:rowOff>
+      <xdr:rowOff>111240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -377,7 +374,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="651240" y="533520"/>
-          <a:ext cx="751680" cy="747720"/>
+          <a:ext cx="751320" cy="747360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -397,24 +394,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="54" zoomScaleNormal="54" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="57.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="18.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="58.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="32.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="18.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="9.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="20.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="11.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="21.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="20.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="11.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="21.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="92.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -430,8 +428,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="5"/>
+      <c r="K1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="24.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3"/>
@@ -444,8 +441,7 @@
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="7"/>
+      <c r="K2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3"/>
@@ -460,8 +456,7 @@
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="9"/>
+      <c r="K3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="40.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
@@ -485,29 +480,26 @@
       <c r="G4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="11" t="s">
         <v>11</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="19.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J18" s="13"/>
+      <c r="I18" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B3:J3"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>